<commit_message>
add place names; sort items by id;
</commit_message>
<xml_diff>
--- a/OctopathTraveler/Resource/info.xlsx
+++ b/OctopathTraveler/Resource/info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Git Projects\OctopathTraveler-SaveDataEditor\OctopathTraveler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Git Projects\OctopathTraveler-SaveDataEditor\OctopathTraveler\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA48015A-A493-4D1B-A52B-A490A63568F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77E09F6-A31F-4D2A-91D8-11DF7FE8AEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27990" windowHeight="16440" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27990" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="character" sheetId="3" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="country" sheetId="4" r:id="rId3"/>
     <sheet name="equipment" sheetId="5" r:id="rId4"/>
     <sheet name="item" sheetId="6" r:id="rId5"/>
-    <sheet name="place" sheetId="8" r:id="rId6"/>
+    <sheet name="place" sheetId="12" r:id="rId6"/>
     <sheet name="enemy_weakness" sheetId="1" r:id="rId7"/>
     <sheet name="tame_monster" sheetId="2" r:id="rId8"/>
     <sheet name="treasure_states" sheetId="11" r:id="rId9"/>
+    <sheet name="place_old" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3613" uniqueCount="1519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3791" uniqueCount="1529">
   <si>
     <t>Highland Ratkin I</t>
   </si>
@@ -4617,6 +4618,39 @@
   </si>
   <si>
     <t>HiddenItem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Amphitheater</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lower Bolderfall</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shrine of the Flamebearer</t>
+  </si>
+  <si>
+    <t>Shrine of the Sage</t>
+  </si>
+  <si>
+    <t>Shrine of the Trader</t>
+  </si>
+  <si>
+    <t>Shrine of the Thunderblade</t>
+  </si>
+  <si>
+    <t>Shrine of the Lady of Grace</t>
+  </si>
+  <si>
+    <t>Shrine of the Healer</t>
+  </si>
+  <si>
+    <t>Shrine of the Prince of Thieves</t>
+  </si>
+  <si>
+    <t>Treasure States ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5341,6 +5375,43 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F72F7F-B564-4A49-BF64-771DD109887F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>657</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3682E17-309E-4223-8A15-872D3AF400E3}">
   <dimension ref="A1:B14"/>
@@ -14002,34 +14073,1990 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F72F7F-B564-4A49-BF64-771DD109887F}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D20EDF-2154-4DD4-840F-AF6A10E76CA6}">
+  <dimension ref="A1:C180"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>657</v>
+    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="43" t="s">
+        <v>629</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>682</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="42">
+        <v>12</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>1514</v>
+      </c>
+      <c r="C2" s="42">
+        <v>1257303</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="42">
+        <v>13</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C3" s="42">
+        <v>1257438</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="42">
+        <v>14</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>1512</v>
+      </c>
+      <c r="C4" s="42">
+        <v>1257573</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="42">
+        <v>15</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C5" s="42">
+        <v>1257708</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="42">
+        <v>16</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C6" s="42">
+        <v>1257843</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A7" s="42">
+        <v>17</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C7" s="42">
+        <v>1257978</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A8" s="42">
+        <v>18</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>1508</v>
+      </c>
+      <c r="C8" s="42">
+        <v>1258113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A9" s="42">
+        <v>19</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C9" s="42">
+        <v>1258248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A10" s="42">
+        <v>20</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C10" s="42">
+        <v>1258383</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A11" s="42">
+        <v>21</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>1505</v>
+      </c>
+      <c r="C11" s="42">
+        <v>1258518</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A12" s="42">
+        <v>22</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>1504</v>
+      </c>
+      <c r="C12" s="42">
+        <v>1258653</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A13" s="42">
+        <v>23</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>1503</v>
+      </c>
+      <c r="C13" s="42">
+        <v>1258788</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A14" s="42">
+        <v>24</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>1502</v>
+      </c>
+      <c r="C14" s="42">
+        <v>1258923</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A15" s="42">
+        <v>25</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C15" s="42">
+        <v>1259058</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A16" s="42">
+        <v>26</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>1500</v>
+      </c>
+      <c r="C16" s="42">
+        <v>1259193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A17" s="42">
+        <v>27</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C17" s="42">
+        <v>1259328</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A18" s="42">
+        <v>28</v>
+      </c>
+      <c r="B18" s="39" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C18" s="42">
+        <v>1259463</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A19" s="42">
+        <v>29</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>1497</v>
+      </c>
+      <c r="C19" s="42">
+        <v>1259598</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A20" s="42">
+        <v>30</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>1496</v>
+      </c>
+      <c r="C20" s="42">
+        <v>1259733</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A21" s="42">
+        <v>31</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>1495</v>
+      </c>
+      <c r="C21" s="42">
+        <v>1259868</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="39">
+        <v>32</v>
+      </c>
+      <c r="B22" s="39" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C22" s="39">
+        <v>1260003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A23" s="42">
+        <v>33</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>1494</v>
+      </c>
+      <c r="C23" s="42">
+        <v>1260138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A24" s="38">
+        <v>34</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>1493</v>
+      </c>
+      <c r="C24" s="38">
+        <v>1260273</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A25" s="38">
+        <v>35</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C25" s="38">
+        <v>1260408</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A26" s="38">
+        <v>36</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>1491</v>
+      </c>
+      <c r="C26" s="38">
+        <v>1260543</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A27" s="38">
+        <v>37</v>
+      </c>
+      <c r="B27" s="35" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C27" s="38">
+        <v>1260678</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A28" s="38">
+        <v>38</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>1489</v>
+      </c>
+      <c r="C28" s="38">
+        <v>1260813</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A29" s="38">
+        <v>39</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>1488</v>
+      </c>
+      <c r="C29" s="38">
+        <v>1260948</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A30" s="38">
+        <v>40</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>1487</v>
+      </c>
+      <c r="C30" s="38">
+        <v>1261083</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17.25" x14ac:dyDescent="0.2">
+      <c r="A31" s="35">
+        <v>41</v>
+      </c>
+      <c r="B31" s="35"/>
+      <c r="C31" s="35">
+        <v>1261218</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A32" s="38">
+        <v>42</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>1486</v>
+      </c>
+      <c r="C32" s="38">
+        <v>1261353</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A33" s="38">
+        <v>43</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>1485</v>
+      </c>
+      <c r="C33" s="38">
+        <v>1261488</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A34" s="38">
+        <v>44</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C34" s="38">
+        <v>1261623</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A35" s="38">
+        <v>45</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C35" s="38">
+        <v>1261758</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A36" s="38">
+        <v>46</v>
+      </c>
+      <c r="B36" s="35" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C36" s="38">
+        <v>1261893</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A37" s="38">
+        <v>47</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>1481</v>
+      </c>
+      <c r="C37" s="38">
+        <v>1262028</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A38" s="38">
+        <v>48</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C38" s="38">
+        <v>1262163</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A39" s="38">
+        <v>49</v>
+      </c>
+      <c r="B39" s="35" t="s">
+        <v>1479</v>
+      </c>
+      <c r="C39" s="38">
+        <v>1262298</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A40" s="38">
+        <v>50</v>
+      </c>
+      <c r="B40" s="35" t="s">
+        <v>1478</v>
+      </c>
+      <c r="C40" s="38">
+        <v>1262433</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A41" s="38">
+        <v>51</v>
+      </c>
+      <c r="B41" s="35" t="s">
+        <v>1477</v>
+      </c>
+      <c r="C41" s="38">
+        <v>1262568</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A42" s="38">
+        <v>52</v>
+      </c>
+      <c r="B42" s="35" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C42" s="38">
+        <v>1262703</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A43" s="38">
+        <v>53</v>
+      </c>
+      <c r="B43" s="35" t="s">
+        <v>1475</v>
+      </c>
+      <c r="C43" s="38">
+        <v>1262838</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A44" s="38">
+        <v>54</v>
+      </c>
+      <c r="B44" s="35" t="s">
+        <v>1474</v>
+      </c>
+      <c r="C44" s="38">
+        <v>1262973</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A45" s="38">
+        <v>55</v>
+      </c>
+      <c r="B45" s="35" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C45" s="38">
+        <v>1263108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A46" s="34">
+        <v>56</v>
+      </c>
+      <c r="B46" s="31" t="s">
+        <v>1472</v>
+      </c>
+      <c r="C46" s="34">
+        <v>1263243</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A47" s="34">
+        <v>57</v>
+      </c>
+      <c r="B47" s="31" t="s">
+        <v>1471</v>
+      </c>
+      <c r="C47" s="34">
+        <v>1263378</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A48" s="34">
+        <v>58</v>
+      </c>
+      <c r="B48" s="31" t="s">
+        <v>1470</v>
+      </c>
+      <c r="C48" s="34">
+        <v>1263513</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A49" s="34">
+        <v>59</v>
+      </c>
+      <c r="B49" s="31" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C49" s="34">
+        <v>1263648</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A50" s="34">
+        <v>60</v>
+      </c>
+      <c r="B50" s="31" t="s">
+        <v>1467</v>
+      </c>
+      <c r="C50" s="34">
+        <v>1263783</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A51" s="34">
+        <v>61</v>
+      </c>
+      <c r="B51" s="31" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C51" s="34">
+        <v>1263918</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A52" s="34">
+        <v>62</v>
+      </c>
+      <c r="B52" s="31" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C52" s="34">
+        <v>1264053</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A53" s="34">
+        <v>63</v>
+      </c>
+      <c r="B53" s="31" t="s">
+        <v>1464</v>
+      </c>
+      <c r="C53" s="34">
+        <v>1264188</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A54" s="34">
+        <v>64</v>
+      </c>
+      <c r="B54" s="31" t="s">
+        <v>1463</v>
+      </c>
+      <c r="C54" s="34">
+        <v>1264323</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A55" s="34">
+        <v>65</v>
+      </c>
+      <c r="B55" s="31" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C55" s="34">
+        <v>1264458</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A56" s="34">
+        <v>66</v>
+      </c>
+      <c r="B56" s="31" t="s">
+        <v>1461</v>
+      </c>
+      <c r="C56" s="34">
+        <v>1264593</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A57" s="34">
+        <v>67</v>
+      </c>
+      <c r="B57" s="31" t="s">
+        <v>1460</v>
+      </c>
+      <c r="C57" s="34">
+        <v>1264728</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A58" s="34">
+        <v>68</v>
+      </c>
+      <c r="B58" s="31" t="s">
+        <v>1459</v>
+      </c>
+      <c r="C58" s="34">
+        <v>1264863</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A59" s="34">
+        <v>69</v>
+      </c>
+      <c r="B59" s="31" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C59" s="34">
+        <v>1264998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A60" s="34">
+        <v>70</v>
+      </c>
+      <c r="B60" s="31" t="s">
+        <v>1457</v>
+      </c>
+      <c r="C60" s="34">
+        <v>1265133</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A61" s="34">
+        <v>71</v>
+      </c>
+      <c r="B61" s="31" t="s">
+        <v>1456</v>
+      </c>
+      <c r="C61" s="34">
+        <v>1265268</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A62" s="34">
+        <v>72</v>
+      </c>
+      <c r="B62" s="31" t="s">
+        <v>1455</v>
+      </c>
+      <c r="C62" s="34">
+        <v>1265403</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A63" s="34">
+        <v>73</v>
+      </c>
+      <c r="B63" s="31" t="s">
+        <v>1454</v>
+      </c>
+      <c r="C63" s="34">
+        <v>1265538</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A64" s="34">
+        <v>74</v>
+      </c>
+      <c r="B64" s="31" t="s">
+        <v>1453</v>
+      </c>
+      <c r="C64" s="34">
+        <v>1265673</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A65" s="34">
+        <v>75</v>
+      </c>
+      <c r="B65" s="31" t="s">
+        <v>1452</v>
+      </c>
+      <c r="C65" s="34">
+        <v>1265808</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A66" s="30">
+        <v>76</v>
+      </c>
+      <c r="B66" s="29" t="s">
+        <v>1451</v>
+      </c>
+      <c r="C66" s="30">
+        <v>1265943</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A67" s="30">
+        <v>77</v>
+      </c>
+      <c r="B67" s="29" t="s">
+        <v>1450</v>
+      </c>
+      <c r="C67" s="30">
+        <v>1266078</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A68" s="30">
+        <v>78</v>
+      </c>
+      <c r="B68" s="29" t="s">
+        <v>1449</v>
+      </c>
+      <c r="C68" s="30">
+        <v>1266213</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A69" s="30">
+        <v>79</v>
+      </c>
+      <c r="B69" s="29" t="s">
+        <v>1448</v>
+      </c>
+      <c r="C69" s="30">
+        <v>1266348</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A70" s="30">
+        <v>80</v>
+      </c>
+      <c r="B70" s="29" t="s">
+        <v>1447</v>
+      </c>
+      <c r="C70" s="30">
+        <v>1266483</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A71" s="30">
+        <v>81</v>
+      </c>
+      <c r="B71" s="29" t="s">
+        <v>1446</v>
+      </c>
+      <c r="C71" s="30">
+        <v>1266618</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A72" s="30">
+        <v>82</v>
+      </c>
+      <c r="B72" s="29" t="s">
+        <v>1445</v>
+      </c>
+      <c r="C72" s="30">
+        <v>1266753</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A73" s="30">
+        <v>83</v>
+      </c>
+      <c r="B73" s="29" t="s">
+        <v>1444</v>
+      </c>
+      <c r="C73" s="30">
+        <v>1266888</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A74" s="30">
+        <v>84</v>
+      </c>
+      <c r="B74" s="29" t="s">
+        <v>1443</v>
+      </c>
+      <c r="C74" s="30">
+        <v>1267023</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A75" s="30">
+        <v>85</v>
+      </c>
+      <c r="B75" s="29" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C75" s="30">
+        <v>1267158</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A76" s="30">
+        <v>86</v>
+      </c>
+      <c r="B76" s="29" t="s">
+        <v>1441</v>
+      </c>
+      <c r="C76" s="30">
+        <v>1267293</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A77" s="30">
+        <v>87</v>
+      </c>
+      <c r="B77" s="29" t="s">
+        <v>1440</v>
+      </c>
+      <c r="C77" s="30">
+        <v>1267428</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A78" s="30">
+        <v>88</v>
+      </c>
+      <c r="B78" s="29" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C78" s="30">
+        <v>1267563</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A79" s="30">
+        <v>89</v>
+      </c>
+      <c r="B79" s="29" t="s">
+        <v>1438</v>
+      </c>
+      <c r="C79" s="30">
+        <v>1267698</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A80" s="30">
+        <v>90</v>
+      </c>
+      <c r="B80" s="29" t="s">
+        <v>1437</v>
+      </c>
+      <c r="C80" s="30">
+        <v>1267833</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A81" s="30">
+        <v>91</v>
+      </c>
+      <c r="B81" s="29" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C81" s="30">
+        <v>1267968</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A82" s="30">
+        <v>92</v>
+      </c>
+      <c r="B82" s="29" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C82" s="30">
+        <v>1268103</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A83" s="30">
+        <v>93</v>
+      </c>
+      <c r="B83" s="29" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C83" s="30">
+        <v>1268238</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A84" s="28">
+        <v>94</v>
+      </c>
+      <c r="B84" s="25" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C84" s="28">
+        <v>1268373</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="17.25" x14ac:dyDescent="0.2">
+      <c r="A85" s="25">
+        <v>95</v>
+      </c>
+      <c r="B85" s="25" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C85" s="25">
+        <v>1268508</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A86" s="28">
+        <v>96</v>
+      </c>
+      <c r="B86" s="25" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C86" s="28">
+        <v>1268643</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A87" s="28">
+        <v>97</v>
+      </c>
+      <c r="B87" s="25" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C87" s="28">
+        <v>1268778</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A88" s="28">
+        <v>98</v>
+      </c>
+      <c r="B88" s="25" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C88" s="28">
+        <v>1268913</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A89" s="28">
+        <v>99</v>
+      </c>
+      <c r="B89" s="25" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C89" s="28">
+        <v>1269048</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A90" s="28">
+        <v>100</v>
+      </c>
+      <c r="B90" s="25" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C90" s="28">
+        <v>1269183</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A91" s="28">
+        <v>101</v>
+      </c>
+      <c r="B91" s="25" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C91" s="28">
+        <v>1269318</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A92" s="28">
+        <v>102</v>
+      </c>
+      <c r="B92" s="25" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C92" s="28">
+        <v>1269453</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A93" s="28">
+        <v>103</v>
+      </c>
+      <c r="B93" s="25" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C93" s="28">
+        <v>1269588</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A94" s="28">
+        <v>104</v>
+      </c>
+      <c r="B94" s="25" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C94" s="28">
+        <v>1269723</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A95" s="28">
+        <v>105</v>
+      </c>
+      <c r="B95" s="25" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C95" s="28">
+        <v>1269858</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A96" s="28">
+        <v>106</v>
+      </c>
+      <c r="B96" s="25" t="s">
+        <v>958</v>
+      </c>
+      <c r="C96" s="28">
+        <v>1269993</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A97" s="28">
+        <v>107</v>
+      </c>
+      <c r="B97" s="25" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C97" s="28">
+        <v>1270128</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A98" s="28">
+        <v>108</v>
+      </c>
+      <c r="B98" s="25" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C98" s="28">
+        <v>1270263</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A99" s="28">
+        <v>109</v>
+      </c>
+      <c r="B99" s="25" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C99" s="28">
+        <v>1270398</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A100" s="28">
+        <v>110</v>
+      </c>
+      <c r="B100" s="25" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C100" s="28">
+        <v>1270533</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A101" s="28">
+        <v>111</v>
+      </c>
+      <c r="B101" s="25" t="s">
+        <v>1418</v>
+      </c>
+      <c r="C101" s="28">
+        <v>1270668</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A102" s="28">
+        <v>112</v>
+      </c>
+      <c r="B102" s="25" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C102" s="28">
+        <v>1270803</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A103" s="28">
+        <v>113</v>
+      </c>
+      <c r="B103" s="25" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C103" s="28">
+        <v>1270938</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A104" s="24">
+        <v>114</v>
+      </c>
+      <c r="B104" s="21" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C104" s="24">
+        <v>1271073</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A105" s="24">
+        <v>115</v>
+      </c>
+      <c r="B105" s="21" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C105" s="24">
+        <v>1271208</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A106" s="24">
+        <v>116</v>
+      </c>
+      <c r="B106" s="21" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C106" s="24">
+        <v>1271343</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A107" s="24">
+        <v>117</v>
+      </c>
+      <c r="B107" s="21" t="s">
+        <v>1412</v>
+      </c>
+      <c r="C107" s="24">
+        <v>1271478</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A108" s="24">
+        <v>118</v>
+      </c>
+      <c r="B108" s="21" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C108" s="24">
+        <v>1271613</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A109" s="24">
+        <v>119</v>
+      </c>
+      <c r="B109" s="21" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C109" s="24">
+        <v>1271748</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A110" s="24">
+        <v>120</v>
+      </c>
+      <c r="B110" s="21" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C110" s="24">
+        <v>1271883</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A111" s="24">
+        <v>121</v>
+      </c>
+      <c r="B111" s="21" t="s">
+        <v>1408</v>
+      </c>
+      <c r="C111" s="24">
+        <v>1272018</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A112" s="24">
+        <v>122</v>
+      </c>
+      <c r="B112" s="21" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C112" s="24">
+        <v>1272153</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A113" s="24">
+        <v>123</v>
+      </c>
+      <c r="B113" s="21" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C113" s="24">
+        <v>1272288</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A114" s="24">
+        <v>124</v>
+      </c>
+      <c r="B114" s="21" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C114" s="24">
+        <v>1272423</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A115" s="24">
+        <v>125</v>
+      </c>
+      <c r="B115" s="21" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C115" s="24">
+        <v>1272558</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A116" s="24">
+        <v>126</v>
+      </c>
+      <c r="B116" s="21" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C116" s="24">
+        <v>1272693</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A117" s="24">
+        <v>127</v>
+      </c>
+      <c r="B117" s="21" t="s">
+        <v>1402</v>
+      </c>
+      <c r="C117" s="24">
+        <v>1272828</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A118" s="24">
+        <v>128</v>
+      </c>
+      <c r="B118" s="21" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C118" s="24">
+        <v>1272963</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A119" s="24">
+        <v>129</v>
+      </c>
+      <c r="B119" s="21" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C119" s="24">
+        <v>1273098</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A120" s="24">
+        <v>130</v>
+      </c>
+      <c r="B120" s="21" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C120" s="24">
+        <v>1273233</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A121" s="24">
+        <v>131</v>
+      </c>
+      <c r="B121" s="21" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C121" s="24">
+        <v>1273368</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A122" s="24">
+        <v>132</v>
+      </c>
+      <c r="B122" s="21" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C122" s="24">
+        <v>1273503</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A123" s="24">
+        <v>133</v>
+      </c>
+      <c r="B123" s="21" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C123" s="24">
+        <v>1273638</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A124" s="24">
+        <v>134</v>
+      </c>
+      <c r="B124" s="21" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C124" s="24">
+        <v>1273773</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A125" s="24">
+        <v>135</v>
+      </c>
+      <c r="B125" s="21" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C125" s="24">
+        <v>1273908</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A126" s="24">
+        <v>136</v>
+      </c>
+      <c r="B126" s="21" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C126" s="24">
+        <v>1274043</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A127" s="20">
+        <v>137</v>
+      </c>
+      <c r="B127" s="17" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C127" s="20">
+        <v>1274178</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A128" s="20">
+        <v>138</v>
+      </c>
+      <c r="B128" s="17" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C128" s="20">
+        <v>1274313</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A129" s="20">
+        <v>139</v>
+      </c>
+      <c r="B129" s="17" t="s">
+        <v>1390</v>
+      </c>
+      <c r="C129" s="20">
+        <v>1274448</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A130" s="20">
+        <v>140</v>
+      </c>
+      <c r="B130" s="17" t="s">
+        <v>1389</v>
+      </c>
+      <c r="C130" s="20">
+        <v>1274583</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A131" s="20">
+        <v>141</v>
+      </c>
+      <c r="B131" s="17" t="s">
+        <v>1388</v>
+      </c>
+      <c r="C131" s="20">
+        <v>1274718</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A132" s="20">
+        <v>142</v>
+      </c>
+      <c r="B132" s="17" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C132" s="20">
+        <v>1274853</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A133" s="20">
+        <v>143</v>
+      </c>
+      <c r="B133" s="17" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C133" s="20">
+        <v>1274988</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A134" s="20">
+        <v>144</v>
+      </c>
+      <c r="B134" s="17" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C134" s="20">
+        <v>1275123</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A135" s="20">
+        <v>145</v>
+      </c>
+      <c r="B135" s="17" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C135" s="20">
+        <v>1275258</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A136" s="20">
+        <v>146</v>
+      </c>
+      <c r="B136" s="17" t="s">
+        <v>1383</v>
+      </c>
+      <c r="C136" s="20">
+        <v>1275393</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A137" s="20">
+        <v>147</v>
+      </c>
+      <c r="B137" s="17" t="s">
+        <v>1381</v>
+      </c>
+      <c r="C137" s="20">
+        <v>1275528</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A138" s="20">
+        <v>148</v>
+      </c>
+      <c r="B138" s="17" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C138" s="20">
+        <v>1275663</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A139" s="20">
+        <v>149</v>
+      </c>
+      <c r="B139" s="17" t="s">
+        <v>1379</v>
+      </c>
+      <c r="C139" s="20">
+        <v>1275798</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A140" s="20">
+        <v>150</v>
+      </c>
+      <c r="B140" s="17" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C140" s="20">
+        <v>1275933</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A141" s="20">
+        <v>151</v>
+      </c>
+      <c r="B141" s="17" t="s">
+        <v>1377</v>
+      </c>
+      <c r="C141" s="20">
+        <v>1276068</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A142" s="20">
+        <v>152</v>
+      </c>
+      <c r="B142" s="17" t="s">
+        <v>1376</v>
+      </c>
+      <c r="C142" s="20">
+        <v>1276203</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A143" s="20">
+        <v>153</v>
+      </c>
+      <c r="B143" s="17" t="s">
+        <v>1375</v>
+      </c>
+      <c r="C143" s="20">
+        <v>1276338</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A144" s="20">
+        <v>154</v>
+      </c>
+      <c r="B144" s="17" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C144" s="20">
+        <v>1276473</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A145" s="20">
+        <v>155</v>
+      </c>
+      <c r="B145" s="17" t="s">
+        <v>1373</v>
+      </c>
+      <c r="C145" s="20">
+        <v>1276608</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A146" s="20">
+        <v>156</v>
+      </c>
+      <c r="B146" s="17" t="s">
+        <v>1372</v>
+      </c>
+      <c r="C146" s="20">
+        <v>1276743</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A147" s="20">
+        <v>157</v>
+      </c>
+      <c r="B147" s="17" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C147" s="20">
+        <v>1276878</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A148" s="14">
+        <v>158</v>
+      </c>
+      <c r="B148" s="11" t="s">
+        <v>1370</v>
+      </c>
+      <c r="C148" s="14">
+        <v>1277013</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A149" s="14">
+        <v>159</v>
+      </c>
+      <c r="B149" s="11" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C149" s="14">
+        <v>1277148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A150" s="14">
+        <v>160</v>
+      </c>
+      <c r="B150" s="11" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C150" s="14">
+        <v>1277283</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A151" s="14">
+        <v>161</v>
+      </c>
+      <c r="B151" s="11" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C151" s="14">
+        <v>1277418</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A152" s="14">
+        <v>162</v>
+      </c>
+      <c r="B152" s="11" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C152" s="14">
+        <v>1277553</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A153" s="14">
+        <v>163</v>
+      </c>
+      <c r="B153" s="11" t="s">
+        <v>1364</v>
+      </c>
+      <c r="C153" s="14">
+        <v>1277688</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A154" s="14">
+        <v>164</v>
+      </c>
+      <c r="B154" s="11" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C154" s="14">
+        <v>1277823</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A155" s="14">
+        <v>165</v>
+      </c>
+      <c r="B155" s="11" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C155" s="14">
+        <v>1277958</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A156" s="14">
+        <v>166</v>
+      </c>
+      <c r="B156" s="11" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C156" s="14">
+        <v>1278093</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A157" s="14">
+        <v>167</v>
+      </c>
+      <c r="B157" s="11" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C157" s="14">
+        <v>1278228</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A158" s="14">
+        <v>168</v>
+      </c>
+      <c r="B158" s="11" t="s">
+        <v>1359</v>
+      </c>
+      <c r="C158" s="14">
+        <v>1278363</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A159" s="14">
+        <v>169</v>
+      </c>
+      <c r="B159" s="11" t="s">
+        <v>1358</v>
+      </c>
+      <c r="C159" s="14">
+        <v>1278498</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A160" s="14">
+        <v>170</v>
+      </c>
+      <c r="B160" s="11" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C160" s="14">
+        <v>1278633</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A161" s="14">
+        <v>171</v>
+      </c>
+      <c r="B161" s="11" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C161" s="14">
+        <v>1278768</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A162" s="14">
+        <v>172</v>
+      </c>
+      <c r="B162" s="11" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C162" s="14">
+        <v>1278903</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A163" s="14">
+        <v>173</v>
+      </c>
+      <c r="B163" s="11" t="s">
+        <v>1353</v>
+      </c>
+      <c r="C163" s="14">
+        <v>1279038</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A164" s="14">
+        <v>174</v>
+      </c>
+      <c r="B164" s="11" t="s">
+        <v>1352</v>
+      </c>
+      <c r="C164" s="14">
+        <v>1279173</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A165" s="14">
+        <v>175</v>
+      </c>
+      <c r="B165" s="11" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C165" s="14">
+        <v>1279308</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A166" s="10">
+        <v>176</v>
+      </c>
+      <c r="B166" s="7"/>
+      <c r="C166" s="10">
+        <v>1280793</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A167" s="10">
+        <v>177</v>
+      </c>
+      <c r="B167" s="7"/>
+      <c r="C167" s="10">
+        <v>1280793</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A168" s="10">
+        <v>178</v>
+      </c>
+      <c r="B168" s="7"/>
+      <c r="C168" s="10">
+        <v>1280793</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A169" s="10">
+        <v>179</v>
+      </c>
+      <c r="B169" s="7" t="s">
+        <v>1521</v>
+      </c>
+      <c r="C169" s="10">
+        <v>1280793</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A170" s="10">
+        <v>180</v>
+      </c>
+      <c r="B170" s="7" t="s">
+        <v>1522</v>
+      </c>
+      <c r="C170" s="10">
+        <v>1280793</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A171" s="10">
+        <v>181</v>
+      </c>
+      <c r="B171" s="7" t="s">
+        <v>1523</v>
+      </c>
+      <c r="C171" s="10">
+        <v>1280793</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A172" s="10">
+        <v>182</v>
+      </c>
+      <c r="B172" s="7" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C172" s="10">
+        <v>1280793</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A173" s="10">
+        <v>183</v>
+      </c>
+      <c r="B173" s="7" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C173" s="10">
+        <v>1280793</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A174" s="10">
+        <v>184</v>
+      </c>
+      <c r="B174" s="7" t="s">
+        <v>1526</v>
+      </c>
+      <c r="C174" s="10">
+        <v>1280793</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A175" s="10">
+        <v>185</v>
+      </c>
+      <c r="B175" s="7" t="s">
+        <v>1527</v>
+      </c>
+      <c r="C175" s="10">
+        <v>1280793</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A176" s="10">
+        <v>186</v>
+      </c>
+      <c r="B176" s="7" t="s">
+        <v>1350</v>
+      </c>
+      <c r="C176" s="10">
+        <v>1280793</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A177" s="10">
+        <v>187</v>
+      </c>
+      <c r="B177" s="7" t="s">
+        <v>1349</v>
+      </c>
+      <c r="C177" s="10">
+        <v>1280928</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A178" s="10">
+        <v>188</v>
+      </c>
+      <c r="B178" s="7" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C178" s="10">
+        <v>1281063</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A179" s="10">
+        <v>189</v>
+      </c>
+      <c r="B179" s="7" t="s">
+        <v>1347</v>
+      </c>
+      <c r="C179" s="10">
+        <v>1281198</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A180" s="10">
+        <v>190</v>
+      </c>
+      <c r="B180" s="7" t="s">
+        <v>1346</v>
+      </c>
+      <c r="C180" s="10">
+        <v>1281333</v>
       </c>
     </row>
   </sheetData>
@@ -26255,8 +28282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E57D94B-C55A-4C17-A133-E7F40059C371}">
   <dimension ref="A1:F170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add "The Gate of Finis" and "Journey's End" place; change error url(About windows);
</commit_message>
<xml_diff>
--- a/OctopathTraveler/Resource/info.xlsx
+++ b/OctopathTraveler/Resource/info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Git Projects\OctopathTraveler-SaveDataEditor\OctopathTraveler\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4BFB06-389C-4B2F-B725-80CCB8405848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9FC69A-1C53-4DF2-82DC-AD17C03E2812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27990" windowHeight="16440" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4623" uniqueCount="1556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4629" uniqueCount="1558">
   <si>
     <t>Highland Ratkin I</t>
   </si>
@@ -4710,10 +4710,6 @@
     <t>#20124D,#D9D2E9</t>
   </si>
   <si>
-    <t>UNKNOWN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Color</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4744,6 +4740,16 @@
   </si>
   <si>
     <t>Index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Gate of Finis</t>
+  </si>
+  <si>
+    <t>Journey's End</t>
+  </si>
+  <si>
+    <t>Don't know the name/(ㄒoㄒ)/~~</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5473,10 +5479,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E57D94B-C55A-4C17-A133-E7F40059C371}">
-  <dimension ref="A1:F180"/>
+  <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="D171" sqref="D171"/>
+    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="B180" sqref="B180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -8428,6 +8434,34 @@
       </c>
       <c r="E180" s="8"/>
       <c r="F180" s="7"/>
+    </row>
+    <row r="181" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A181" s="10">
+        <v>1282008</v>
+      </c>
+      <c r="B181" s="7" t="s">
+        <v>1555</v>
+      </c>
+      <c r="C181" s="7">
+        <v>0</v>
+      </c>
+      <c r="D181" s="7"/>
+      <c r="E181" s="10"/>
+      <c r="F181" s="10"/>
+    </row>
+    <row r="182" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A182" s="10">
+        <v>1282143</v>
+      </c>
+      <c r="B182" s="7" t="s">
+        <v>1556</v>
+      </c>
+      <c r="C182" s="7">
+        <v>0</v>
+      </c>
+      <c r="D182" s="7"/>
+      <c r="E182" s="10"/>
+      <c r="F182" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -12735,7 +12769,7 @@
         <v>137</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
@@ -17121,10 +17155,10 @@
         <v>679</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -18756,7 +18790,7 @@
         <v>137</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="C118" s="46">
         <v>1</v>
@@ -20352,7 +20386,7 @@
         <v>1318</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="C232" s="46">
         <v>5</v>
@@ -21892,7 +21926,7 @@
         <v>1715</v>
       </c>
       <c r="B342" s="2" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="C342" s="46">
         <v>9</v>
@@ -22984,7 +23018,7 @@
         <v>0</v>
       </c>
       <c r="B420" s="2" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="C420" s="46">
         <v>11</v>
@@ -23250,7 +23284,7 @@
         <v>1921</v>
       </c>
       <c r="B439" s="2" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="C439" s="46">
         <v>11</v>
@@ -25434,7 +25468,7 @@
         <v>844</v>
       </c>
       <c r="B595" s="2" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="C595" s="2">
         <v>14</v>
@@ -26022,7 +26056,7 @@
         <v>0</v>
       </c>
       <c r="B637" s="2" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="C637" s="2">
         <v>14</v>
@@ -26124,10 +26158,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D20EDF-2154-4DD4-840F-AF6A10E76CA6}">
-  <dimension ref="A1:D183"/>
+  <dimension ref="A1:D185"/>
   <sheetViews>
-    <sheetView topLeftCell="A182" workbookViewId="0">
-      <selection activeCell="D198" sqref="D198"/>
+    <sheetView topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="B183" sqref="B183:B184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -26145,7 +26179,7 @@
         <v>679</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="D1" s="43" t="s">
         <v>1525</v>
@@ -28646,7 +28680,7 @@
         <v>193</v>
       </c>
       <c r="B181" s="10" t="s">
-        <v>1545</v>
+        <v>1557</v>
       </c>
       <c r="C181" s="7" t="s">
         <v>1544</v>
@@ -28660,7 +28694,7 @@
         <v>194</v>
       </c>
       <c r="B182" s="10" t="s">
-        <v>1545</v>
+        <v>1557</v>
       </c>
       <c r="C182" s="7" t="s">
         <v>1544</v>
@@ -28671,15 +28705,43 @@
     </row>
     <row r="183" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A183" s="10">
-        <v>199</v>
-      </c>
-      <c r="B183" s="10" t="s">
-        <v>1545</v>
+        <v>195</v>
+      </c>
+      <c r="B183" s="7" t="s">
+        <v>1555</v>
       </c>
       <c r="C183" s="7" t="s">
         <v>1544</v>
       </c>
       <c r="D183" s="10">
+        <v>1282008</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A184" s="10">
+        <v>196</v>
+      </c>
+      <c r="B184" s="7" t="s">
+        <v>1556</v>
+      </c>
+      <c r="C184" s="7" t="s">
+        <v>1544</v>
+      </c>
+      <c r="D184" s="10">
+        <v>1282143</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A185" s="10">
+        <v>199</v>
+      </c>
+      <c r="B185" s="10" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C185" s="7" t="s">
+        <v>1544</v>
+      </c>
+      <c r="D185" s="10">
         <v>1282548</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add  the item id for "Spurning Ribbon";
</commit_message>
<xml_diff>
--- a/OctopathTraveler/Resource/info.xlsx
+++ b/OctopathTraveler/Resource/info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Git Projects\OctopathTraveler-SaveDataEditor\OctopathTraveler\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9FC69A-1C53-4DF2-82DC-AD17C03E2812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9756EEAE-15AE-4CA9-BE05-5D8A4AC4C074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27990" windowHeight="16440" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27990" windowHeight="16440" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="character" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4629" uniqueCount="1558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4630" uniqueCount="1559">
   <si>
     <t>Highland Ratkin I</t>
   </si>
@@ -4750,6 +4750,10 @@
   </si>
   <si>
     <t>Don't know the name/(ㄒoㄒ)/~~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spurning Ribbon</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5481,8 +5485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E57D94B-C55A-4C17-A133-E7F40059C371}">
   <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="B180" sqref="B180"/>
+    <sheetView topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="B167" sqref="B167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -11807,10 +11811,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7ADF300-C656-4AE5-97E2-7AF6BFE7A158}">
-  <dimension ref="A1:B663"/>
+  <dimension ref="A1:B664"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
+    <sheetView topLeftCell="A575" workbookViewId="0">
+      <selection activeCell="B582" sqref="B582"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -16470,657 +16474,665 @@
     </row>
     <row r="582" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A582" s="3">
-        <v>1903</v>
-      </c>
-      <c r="B582" s="3" t="s">
-        <v>1246</v>
+        <v>1901</v>
+      </c>
+      <c r="B582" s="2" t="s">
+        <v>1548</v>
       </c>
     </row>
     <row r="583" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A583" s="3">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="B583" s="3" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="584" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A584" s="3">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="B584" s="3" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="585" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A585" s="3">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="B585" s="3" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="586" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A586" s="3">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="B586" s="3" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="587" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A587" s="3">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="B587" s="3" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="588" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A588" s="3">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="B588" s="3" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="589" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A589" s="3">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="B589" s="3" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A590" s="3">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="B590" s="3" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A591" s="3">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="B591" s="3" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A592" s="3">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="B592" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A593" s="3">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="B593" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A594" s="3">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="B594" s="3" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A595" s="3">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="B595" s="3" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A596" s="3">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="B596" s="3" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A597" s="3">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="B597" s="3" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A598" s="3">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="B598" s="3" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A599" s="3">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="B599" s="3" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A600" s="3">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="B600" s="3" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A601" s="3">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="B601" s="3" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A602" s="3">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="B602" s="3" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A603" s="3">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="B603" s="3" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A604" s="3">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="B604" s="3" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A605" s="3">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="B605" s="3" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A606" s="3">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="B606" s="3" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="607" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A607" s="3">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="B607" s="3" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A608" s="3">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="B608" s="3" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A609" s="3">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="B609" s="3" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A610" s="3">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="B610" s="3" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A611" s="3">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="B611" s="3" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A612" s="3">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="B612" s="3" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A613" s="3">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="B613" s="3" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="614" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A614" s="3">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="B614" s="3" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="615" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A615" s="3">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="B615" s="3" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A616" s="3">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="B616" s="3" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A617" s="3">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="B617" s="3" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A618" s="3">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="B618" s="3" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A619" s="3">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="B619" s="3" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A620" s="3">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="B620" s="3" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A621" s="3">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="B621" s="3" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A622" s="3">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="B622" s="3" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A623" s="3">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="B623" s="3" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A624" s="3">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="B624" s="3" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="625" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A625" s="3">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="B625" s="3" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="626" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A626" s="3">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="B626" s="3" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A627" s="3">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="B627" s="3" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A628" s="3">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="B628" s="3" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="629" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A629" s="3">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="B629" s="3" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="630" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A630" s="3">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="B630" s="3" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="631" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A631" s="3">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="B631" s="3" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="632" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A632" s="3">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="B632" s="3" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="633" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A633" s="3">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="B633" s="3" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="634" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A634" s="3">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="B634" s="3" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="635" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A635" s="3">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="B635" s="3" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="636" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A636" s="3">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="B636" s="3" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="637" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A637" s="3">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="B637" s="3" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A638" s="3">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="B638" s="3" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="639" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A639" s="3">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="B639" s="3" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A640" s="3">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="B640" s="3" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A641" s="3">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="B641" s="3" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A642" s="3">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="B642" s="3" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A643" s="3">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="B643" s="3" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A644" s="3">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="B644" s="3" t="s">
-        <v>1339</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A645" s="3">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="B645" s="3" t="s">
-        <v>1308</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A646" s="3">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="B646" s="3" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A647" s="3">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="B647" s="3" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A648" s="3">
-        <v>2500</v>
+        <v>1968</v>
       </c>
       <c r="B648" s="3" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A649" s="3">
-        <v>2501</v>
+        <v>2500</v>
       </c>
       <c r="B649" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A650" s="3">
-        <v>2502</v>
+        <v>2501</v>
       </c>
       <c r="B650" s="3" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A651" s="3">
-        <v>2503</v>
+        <v>2502</v>
       </c>
       <c r="B651" s="3" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A652" s="3">
-        <v>2504</v>
+        <v>2503</v>
       </c>
       <c r="B652" s="3" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A653" s="3">
-        <v>2505</v>
+        <v>2504</v>
       </c>
       <c r="B653" s="3" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A654" s="3">
-        <v>2506</v>
+        <v>2505</v>
       </c>
       <c r="B654" s="3" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A655" s="3">
-        <v>2507</v>
+        <v>2506</v>
       </c>
       <c r="B655" s="3" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A656" s="3">
-        <v>2516</v>
+        <v>2507</v>
       </c>
       <c r="B656" s="3" t="s">
-        <v>649</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A657" s="3">
-        <v>2517</v>
+        <v>2516</v>
       </c>
       <c r="B657" s="3" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A658" s="3">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="B658" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A659" s="3">
-        <v>2519</v>
+        <v>2518</v>
       </c>
       <c r="B659" s="3" t="s">
-        <v>1319</v>
+        <v>651</v>
       </c>
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A660" s="3">
-        <v>2520</v>
+        <v>2519</v>
       </c>
       <c r="B660" s="3" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A661" s="3">
-        <v>2521</v>
+        <v>2520</v>
       </c>
       <c r="B661" s="3" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A662" s="3">
-        <v>2522</v>
+        <v>2521</v>
       </c>
       <c r="B662" s="3" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A663" s="3">
+        <v>2522</v>
+      </c>
+      <c r="B663" s="3" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="664" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A664" s="3">
         <v>2523</v>
       </c>
-      <c r="B663" s="3" t="s">
+      <c r="B664" s="3" t="s">
         <v>1323</v>
       </c>
     </row>
@@ -17134,8 +17146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C8762B1-6AF5-413F-9B69-EB32F415BE08}">
   <dimension ref="A1:E643"/>
   <sheetViews>
-    <sheetView topLeftCell="A495" workbookViewId="0">
-      <selection activeCell="I509" sqref="I509"/>
+    <sheetView tabSelected="1" topLeftCell="A417" workbookViewId="0">
+      <selection activeCell="E423" sqref="E423"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -23015,10 +23027,10 @@
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A420" s="3">
-        <v>0</v>
+        <v>1901</v>
       </c>
       <c r="B420" s="2" t="s">
-        <v>1548</v>
+        <v>1558</v>
       </c>
       <c r="C420" s="46">
         <v>11</v>

</xml_diff>